<commit_message>
fixed errors in the spreadsheet that were causing issues with the code
</commit_message>
<xml_diff>
--- a/company_data/sample/Week_Day Treasury Rates.xlsx
+++ b/company_data/sample/Week_Day Treasury Rates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10600" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="Rates" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1494"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1467" workbookViewId="0">
+      <selection activeCell="B1500" sqref="B1500"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -523,8 +525,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <f>B4-1</f>
-        <v>40955</v>
+        <v>40959</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1510,8 +1511,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="1">
-        <f>B40+1</f>
-        <v>41009</v>
+        <v>41005</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2555,8 +2555,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="1">
-        <f>B74-1</f>
-        <v>41053</v>
+        <v>41057</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3339,8 +3338,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="1">
-        <f>B101-1</f>
-        <v>41092</v>
+        <v>41094</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -4587,8 +4585,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="1">
-        <f>B144-1</f>
-        <v>41151</v>
+        <v>41155</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -5313,8 +5310,7 @@
         <v>0</v>
       </c>
       <c r="B170" s="1">
-        <f>B169-1</f>
-        <v>41186</v>
+        <v>41190</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -6039,8 +6035,7 @@
         <v>0</v>
       </c>
       <c r="B195" s="1">
-        <f>B194-1</f>
-        <v>41221</v>
+        <v>41225</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -6272,8 +6267,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="1">
-        <f>B202-1</f>
-        <v>41233</v>
+        <v>41235</v>
       </c>
       <c r="C203">
         <v>0</v>
@@ -6940,8 +6934,7 @@
         <v>4</v>
       </c>
       <c r="B226" s="1">
-        <f>B225-1</f>
-        <v>41266</v>
+        <v>41268</v>
       </c>
       <c r="C226">
         <v>0</v>
@@ -7086,8 +7079,7 @@
         <v>4</v>
       </c>
       <c r="B231" s="1">
-        <f>B230-1</f>
-        <v>41273</v>
+        <v>41275</v>
       </c>
       <c r="C231">
         <v>0</v>
@@ -7493,8 +7485,7 @@
         <v>0</v>
       </c>
       <c r="B245" s="1">
-        <f>B244-1</f>
-        <v>41291</v>
+        <v>41295</v>
       </c>
       <c r="C245">
         <v>0</v>
@@ -8074,8 +8065,7 @@
         <v>0</v>
       </c>
       <c r="B265" s="1">
-        <f>B264-1</f>
-        <v>41319</v>
+        <v>41323</v>
       </c>
       <c r="C265">
         <v>0</v>
@@ -8916,8 +8906,7 @@
         <v>1</v>
       </c>
       <c r="B294" s="1">
-        <f>B295+1</f>
-        <v>41366</v>
+        <v>41362</v>
       </c>
       <c r="C294">
         <v>0</v>
@@ -10106,8 +10095,7 @@
         <v>0</v>
       </c>
       <c r="B335" s="1">
-        <f>B334-1</f>
-        <v>41417</v>
+        <v>41421</v>
       </c>
       <c r="C335">
         <v>0</v>
@@ -10919,8 +10907,7 @@
         <v>2</v>
       </c>
       <c r="B363" s="1">
-        <f>B362-1</f>
-        <v>41457</v>
+        <v>41459</v>
       </c>
       <c r="C363">
         <v>0</v>
@@ -12138,8 +12125,7 @@
         <v>0</v>
       </c>
       <c r="B405" s="1">
-        <f>B404-1</f>
-        <v>41515</v>
+        <v>41519</v>
       </c>
       <c r="C405">
         <v>0</v>
@@ -13009,8 +12995,7 @@
         <v>0</v>
       </c>
       <c r="B435" s="1">
-        <f>B434-1</f>
-        <v>41557</v>
+        <v>41561</v>
       </c>
       <c r="C435">
         <v>0</v>
@@ -13590,8 +13575,7 @@
         <v>0</v>
       </c>
       <c r="B455" s="1">
-        <f>B454-1</f>
-        <v>41585</v>
+        <v>41589</v>
       </c>
       <c r="C455">
         <v>0</v>
@@ -13968,8 +13952,7 @@
         <v>2</v>
       </c>
       <c r="B468" s="1">
-        <f>B467-1</f>
-        <v>41604</v>
+        <v>41606</v>
       </c>
       <c r="C468">
         <v>0</v>
@@ -14520,8 +14503,7 @@
         <v>3</v>
       </c>
       <c r="B487" s="1">
-        <f>B486-1</f>
-        <v>41631</v>
+        <v>41633</v>
       </c>
       <c r="C487">
         <v>0</v>
@@ -14666,8 +14648,7 @@
         <v>3</v>
       </c>
       <c r="B492" s="1">
-        <f>B491-1</f>
-        <v>41638</v>
+        <v>41640</v>
       </c>
       <c r="C492">
         <v>0</v>
@@ -15044,8 +15025,7 @@
         <v>0</v>
       </c>
       <c r="B505" s="1">
-        <f>B504-1</f>
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="C505">
         <v>0</v>
@@ -15625,8 +15605,7 @@
         <v>0</v>
       </c>
       <c r="B525" s="1">
-        <f>B524-1</f>
-        <v>41683</v>
+        <v>43148</v>
       </c>
       <c r="C525">
         <v>0</v>
@@ -16841,53 +16820,52 @@
     </row>
     <row r="567" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B567" s="1">
-        <f>B568-1</f>
-        <v>41744</v>
+        <v>41745</v>
       </c>
       <c r="C567">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="D567">
-        <v>0</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E567">
-        <v>0</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="G567">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>2.8000000000000003E-4</v>
       </c>
       <c r="H567">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>5.2999999999999998E-4</v>
       </c>
       <c r="I567">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>8.8999999999999995E-4</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B568" s="1">
-        <v>41745</v>
+        <v>41746</v>
       </c>
       <c r="C568">
-        <v>2.8000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D568">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E568">
-        <v>8.8999999999999996E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="G568">
         <f t="shared" si="25"/>
-        <v>2.8000000000000003E-4</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="H568">
         <f t="shared" si="26"/>
@@ -16895,36 +16873,36 @@
       </c>
       <c r="I568">
         <f t="shared" si="27"/>
-        <v>8.8999999999999995E-4</v>
+        <v>9.3999999999999997E-4</v>
       </c>
     </row>
     <row r="569" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B569" s="1">
-        <v>41746</v>
+        <v>41747</v>
       </c>
       <c r="C569">
-        <v>2.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="D569">
-        <v>5.2999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E569">
-        <v>9.4E-2</v>
+        <v>0</v>
       </c>
       <c r="G569">
-        <f t="shared" si="25"/>
-        <v>2.5000000000000001E-4</v>
+        <f>C569/100</f>
+        <v>0</v>
       </c>
       <c r="H569">
-        <f t="shared" si="26"/>
-        <v>5.2999999999999998E-4</v>
+        <f>D569/100</f>
+        <v>0</v>
       </c>
       <c r="I569">
-        <f t="shared" si="27"/>
-        <v>9.3999999999999997E-4</v>
+        <f>E569/100</f>
+        <v>0</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.2">
@@ -17657,8 +17635,7 @@
         <v>0</v>
       </c>
       <c r="B595" s="1">
-        <f>B594-1</f>
-        <v>41781</v>
+        <v>41785</v>
       </c>
       <c r="C595">
         <v>0</v>
@@ -18499,8 +18476,7 @@
         <v>1</v>
       </c>
       <c r="B624" s="1">
-        <f>B625+1</f>
-        <v>41828</v>
+        <v>41824</v>
       </c>
       <c r="C624">
         <v>0</v>
@@ -19689,8 +19665,7 @@
         <v>0</v>
       </c>
       <c r="B665" s="1">
-        <f>B664-1</f>
-        <v>41879</v>
+        <v>41883</v>
       </c>
       <c r="C665">
         <v>0</v>
@@ -20560,8 +20535,7 @@
         <v>0</v>
       </c>
       <c r="B695" s="1">
-        <f>B694-1</f>
-        <v>41921</v>
+        <v>41925</v>
       </c>
       <c r="C695">
         <v>0</v>
@@ -21170,8 +21144,7 @@
         <v>4</v>
       </c>
       <c r="B716" s="1">
-        <f>B715-1</f>
-        <v>41952</v>
+        <v>41954</v>
       </c>
       <c r="C716">
         <v>0</v>
@@ -21519,8 +21492,7 @@
         <v>2</v>
       </c>
       <c r="B728" s="1">
-        <f>B727-1</f>
-        <v>41968</v>
+        <v>41960</v>
       </c>
       <c r="C728">
         <v>0</v>
@@ -22100,8 +22072,7 @@
         <v>2</v>
       </c>
       <c r="B748" s="1">
-        <f>B747-1</f>
-        <v>41996</v>
+        <v>41968</v>
       </c>
       <c r="C748">
         <v>0</v>
@@ -22246,8 +22217,7 @@
         <v>2</v>
       </c>
       <c r="B753" s="1">
-        <f>B752-1</f>
-        <v>42003</v>
+        <v>42005</v>
       </c>
       <c r="C753">
         <v>0</v>
@@ -22595,8 +22565,7 @@
         <v>0</v>
       </c>
       <c r="B765" s="1">
-        <f>B764-1</f>
-        <v>42019</v>
+        <v>42023</v>
       </c>
       <c r="C765">
         <v>0</v>
@@ -23176,8 +23145,7 @@
         <v>0</v>
       </c>
       <c r="B785" s="1">
-        <f>B784-1</f>
-        <v>42047</v>
+        <v>42051</v>
       </c>
       <c r="C785">
         <v>0</v>
@@ -24163,8 +24131,7 @@
         <v>1</v>
       </c>
       <c r="B819" s="1">
-        <f>B820+1</f>
-        <v>42101</v>
+        <v>42097</v>
       </c>
       <c r="C819">
         <v>0</v>
@@ -25208,8 +25175,7 @@
         <v>0</v>
       </c>
       <c r="B855" s="1">
-        <f>B854-1</f>
-        <v>42145</v>
+        <v>42149</v>
       </c>
       <c r="C855">
         <v>0</v>
@@ -26050,8 +26016,7 @@
         <v>1</v>
       </c>
       <c r="B884" s="1">
-        <f>B885+1</f>
-        <v>42192</v>
+        <v>42188</v>
       </c>
       <c r="C884">
         <v>0</v>
@@ -27385,8 +27350,7 @@
         <v>0</v>
       </c>
       <c r="B930" s="1">
-        <f>B929-1</f>
-        <v>42250</v>
+        <v>42254</v>
       </c>
       <c r="C930">
         <v>0</v>
@@ -28111,8 +28075,7 @@
         <v>0</v>
       </c>
       <c r="B955" s="1">
-        <f>B954-1</f>
-        <v>42285</v>
+        <v>42289</v>
       </c>
       <c r="C955">
         <v>0</v>
@@ -28750,8 +28713,7 @@
         <v>3</v>
       </c>
       <c r="B977" s="1">
-        <f>B976-1</f>
-        <v>42317</v>
+        <v>42319</v>
       </c>
       <c r="C977">
         <v>0</v>
@@ -29070,8 +29032,7 @@
         <v>2</v>
       </c>
       <c r="B988" s="1">
-        <f>B987-1</f>
-        <v>42332</v>
+        <v>42334</v>
       </c>
       <c r="C988">
         <v>0</v>
@@ -29680,8 +29641,7 @@
         <v>1</v>
       </c>
       <c r="B1009" s="1">
-        <f>B1010+1</f>
-        <v>42367</v>
+        <v>42363</v>
       </c>
       <c r="C1009">
         <v>0</v>
@@ -29826,8 +29786,7 @@
         <v>1</v>
       </c>
       <c r="B1014" s="1">
-        <f>B1015+1</f>
-        <v>42374</v>
+        <v>42370</v>
       </c>
       <c r="C1014">
         <v>0</v>
@@ -30146,8 +30105,7 @@
         <v>0</v>
       </c>
       <c r="B1025" s="1">
-        <f>B1024-1</f>
-        <v>42383</v>
+        <v>42387</v>
       </c>
       <c r="C1025">
         <v>0</v>
@@ -30727,8 +30685,7 @@
         <v>0</v>
       </c>
       <c r="B1045" s="1">
-        <f>B1044-1</f>
-        <v>42411</v>
+        <v>42415</v>
       </c>
       <c r="C1045">
         <v>0</v>
@@ -31569,8 +31526,7 @@
         <v>1</v>
       </c>
       <c r="B1074" s="1">
-        <f>B1075+1</f>
-        <v>42458</v>
+        <v>42454</v>
       </c>
       <c r="C1074">
         <v>0</v>
@@ -32904,8 +32860,7 @@
         <v>0</v>
       </c>
       <c r="B1120" s="1">
-        <f>B1119-1</f>
-        <v>42516</v>
+        <v>42520</v>
       </c>
       <c r="C1120">
         <v>0</v>
@@ -33630,8 +33585,7 @@
         <v>0</v>
       </c>
       <c r="B1145" s="1">
-        <f>B1144-1</f>
-        <v>42551</v>
+        <v>42555</v>
       </c>
       <c r="C1145">
         <v>0</v>
@@ -34936,8 +34890,7 @@
         <v>0</v>
       </c>
       <c r="B1190" s="1">
-        <f>B1189-1</f>
-        <v>42614</v>
+        <v>42618</v>
       </c>
       <c r="C1190">
         <v>0</v>
@@ -35662,8 +35615,7 @@
         <v>0</v>
       </c>
       <c r="B1215" s="1">
-        <f>B1214-1</f>
-        <v>42649</v>
+        <v>42653</v>
       </c>
       <c r="C1215">
         <v>0</v>
@@ -36359,8 +36311,7 @@
         <v>1</v>
       </c>
       <c r="B1239" s="1">
-        <f>B1240+1</f>
-        <v>42689</v>
+        <v>42685</v>
       </c>
       <c r="C1239">
         <v>0</v>
@@ -36621,8 +36572,7 @@
         <v>2</v>
       </c>
       <c r="B1248" s="1">
-        <f>B1247-1</f>
-        <v>42696</v>
+        <v>42698</v>
       </c>
       <c r="C1248">
         <v>0</v>
@@ -37260,8 +37210,7 @@
         <v>0</v>
       </c>
       <c r="B1270" s="1">
-        <f>B1269-1</f>
-        <v>42726</v>
+        <v>42730</v>
       </c>
       <c r="C1270">
         <v>0</v>
@@ -37406,8 +37355,7 @@
         <v>0</v>
       </c>
       <c r="B1275" s="1">
-        <f>B1274-1</f>
-        <v>42733</v>
+        <v>42737</v>
       </c>
       <c r="C1275">
         <v>0</v>
@@ -37697,8 +37645,7 @@
         <v>0</v>
       </c>
       <c r="B1285" s="1">
-        <f>B1284-1</f>
-        <v>42747</v>
+        <v>42751</v>
       </c>
       <c r="C1285">
         <v>0</v>
@@ -38423,8 +38370,7 @@
         <v>0</v>
       </c>
       <c r="B1310" s="1">
-        <f>B1309-1</f>
-        <v>42782</v>
+        <v>42786</v>
       </c>
       <c r="C1310">
         <v>0</v>
@@ -39555,8 +39501,7 @@
         <v>1</v>
       </c>
       <c r="B1349" s="1">
-        <f>B1350+1</f>
-        <v>42843</v>
+        <v>42839</v>
       </c>
       <c r="C1349">
         <v>0</v>
@@ -40455,8 +40400,7 @@
         <v>8</v>
       </c>
       <c r="B1380" s="1">
-        <f>B1379-1</f>
-        <v>42880</v>
+        <v>42884</v>
       </c>
       <c r="C1380">
         <v>0</v>
@@ -41210,8 +41154,7 @@
         <v>9</v>
       </c>
       <c r="B1406" s="1">
-        <f>B1405-1</f>
-        <v>42918</v>
+        <v>42920</v>
       </c>
       <c r="C1406">
         <v>0</v>
@@ -42487,8 +42430,7 @@
         <v>8</v>
       </c>
       <c r="B1450" s="1">
-        <f>B1449-1</f>
-        <v>42978</v>
+        <v>42982</v>
       </c>
       <c r="C1450">
         <v>0</v>
@@ -43213,8 +43155,7 @@
         <v>8</v>
       </c>
       <c r="B1475" s="1">
-        <f>B1474-1</f>
-        <v>43013</v>
+        <v>43017</v>
       </c>
       <c r="C1475">
         <v>0</v>

</xml_diff>